<commit_message>
update code table result prediction
</commit_message>
<xml_diff>
--- a/Model and data/Thakek-Mekong_demo.xlsx
+++ b/Model and data/Thakek-Mekong_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOAN\DeployMode-Excel\Model and data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD44EFB6-CFFA-403B-859C-D1BDD7062DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7C0660-168A-4971-9970-E0089DFA8B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,24 +34,6 @@
     <t>Rainfall_w3</t>
   </si>
   <si>
-    <t>Hnk(t-2)</t>
-  </si>
-  <si>
-    <t>Hnk(t-1)</t>
-  </si>
-  <si>
-    <t>Hnk(t)</t>
-  </si>
-  <si>
-    <t>Htk(t-2)</t>
-  </si>
-  <si>
-    <t>Htk(t-1)</t>
-  </si>
-  <si>
-    <t>Htk(t)</t>
-  </si>
-  <si>
     <t>H(t+5)</t>
   </si>
   <si>
@@ -110,6 +92,24 @@
   </si>
   <si>
     <t>10/31/2000</t>
+  </si>
+  <si>
+    <t>Hnk_t2</t>
+  </si>
+  <si>
+    <t>Hnk_t1</t>
+  </si>
+  <si>
+    <t>Hnk_t</t>
+  </si>
+  <si>
+    <t>Htk_t2</t>
+  </si>
+  <si>
+    <t>Htk_t1</t>
+  </si>
+  <si>
+    <t>Htk_t</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -479,30 +479,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0.38</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0.76</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0.85</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0.83</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0.6</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>2.0699999999999998</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>2.8</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>2.61</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0.73</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>0.01</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>0.01</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>0.01</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>0</v>

</xml_diff>